<commit_message>
added edit functions, v1 stylings complete
</commit_message>
<xml_diff>
--- a/Lifehistory/Seabird Key.xlsx
+++ b/Lifehistory/Seabird Key.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LifeHistory\Lifehistory\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="30" windowWidth="22995" windowHeight="10050"/>
   </bookViews>
@@ -54,9 +59,6 @@
     <t>cm</t>
   </si>
   <si>
-    <t>Incubtaion Period</t>
-  </si>
-  <si>
     <t>Fledging Period</t>
   </si>
   <si>
@@ -256,12 +258,15 @@
   </si>
   <si>
     <t>Hatchling Type</t>
+  </si>
+  <si>
+    <t>Incubation Period</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -324,6 +329,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -371,7 +379,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -404,9 +412,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -439,6 +464,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -617,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,7 +692,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -658,13 +700,13 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -675,7 +717,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -686,7 +728,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -707,350 +749,350 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
         <v>14</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
         <v>16</v>
       </c>
-      <c r="B13" t="s">
-        <v>17</v>
-      </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" t="s">
         <v>18</v>
-      </c>
-      <c r="C14" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" t="s">
         <v>23</v>
-      </c>
-      <c r="C16" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" t="s">
         <v>25</v>
-      </c>
-      <c r="C17" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
         <v>27</v>
-      </c>
-      <c r="B19" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" t="s">
         <v>30</v>
-      </c>
-      <c r="C21" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" t="s">
         <v>35</v>
-      </c>
-      <c r="C25" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" t="s">
         <v>38</v>
-      </c>
-      <c r="B28" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" t="s">
         <v>43</v>
-      </c>
-      <c r="B31" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B36" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B44" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="D44" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="E44" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="F44" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F44" s="2" t="s">
+      <c r="G44" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C45" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D45" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E45" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F45" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G45" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C46" t="s">
+        <v>71</v>
+      </c>
+      <c r="D46" t="s">
+        <v>61</v>
+      </c>
+      <c r="E46" t="s">
+        <v>73</v>
+      </c>
+      <c r="F46" t="s">
+        <v>76</v>
+      </c>
+      <c r="G46" t="s">
         <v>72</v>
-      </c>
-      <c r="D46" t="s">
-        <v>62</v>
-      </c>
-      <c r="E46" t="s">
-        <v>74</v>
-      </c>
-      <c r="F46" t="s">
-        <v>77</v>
-      </c>
-      <c r="G46" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C47" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D47" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E47" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F47" t="s">
+        <v>76</v>
+      </c>
+      <c r="G47" t="s">
         <v>77</v>
-      </c>
-      <c r="G47" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C48" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D48" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E48" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F48" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G48" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C49" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D49" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E49" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F49" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G49" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C50" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E50" t="s">
+        <v>75</v>
+      </c>
+      <c r="F50" t="s">
         <v>76</v>
       </c>
-      <c r="F50" t="s">
-        <v>77</v>
-      </c>
       <c r="G50" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D51" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E51" t="s">
+        <v>75</v>
+      </c>
+      <c r="F51" t="s">
         <v>76</v>
       </c>
-      <c r="F51" t="s">
-        <v>77</v>
-      </c>
       <c r="G51" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
+        <v>68</v>
+      </c>
+      <c r="C52" t="s">
+        <v>72</v>
+      </c>
+      <c r="D52" t="s">
         <v>69</v>
       </c>
-      <c r="C52" t="s">
-        <v>73</v>
-      </c>
-      <c r="D52" t="s">
-        <v>70</v>
-      </c>
       <c r="E52" t="s">
+        <v>75</v>
+      </c>
+      <c r="F52" t="s">
         <v>76</v>
       </c>
-      <c r="F52" t="s">
-        <v>77</v>
-      </c>
       <c r="G52" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>